<commit_message>
1.Added ie, firefox, Opera, edge browser 2.Added code for that in Utility 3.Added path in config file 4.Added test data according to that
</commit_message>
<xml_diff>
--- a/Testdata/Login.xlsx
+++ b/Testdata/Login.xlsx
@@ -1,41 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\Testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF5F17-94F6-4095-9F07-16728C7238B6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+  <si>
+    <t>Sno</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Email to send</t>
+  </si>
+  <si>
+    <t>StausofMessage</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>http://newon.docagent.net</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>ddi</t>
+  </si>
+  <si>
+    <t>vinaytalkin@yahoo.com</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Firefox</t>
+  </si>
+  <si>
+    <t>Ie</t>
+  </si>
+  <si>
+    <t>Opera</t>
+  </si>
+  <si>
+    <t>Edgebrowser</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,18 +115,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -328,111 +401,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="4.28515625"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" width="26"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" width="10"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="9.42578125"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="22.7109375"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" width="15.42578125"/>
-    <col bestFit="1" customWidth="1" max="8" min="8" width="14.140625"/>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Sno</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Browser</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>URL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Username</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Password</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Email to send</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>StausofMessage</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Results</t>
-        </is>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Chrome</t>
-        </is>
-      </c>
-      <c r="C2" s="1" t="inlineStr">
-        <is>
-          <t>http://newon.docagent.net</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ddi</t>
-        </is>
-      </c>
-      <c r="F2" s="1" t="inlineStr">
-        <is>
-          <t>vinaytalkin@yahoo.com</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="http://newon.docagent.net/" ref="C2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" display="http://newon.docagent.net/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C3" r:id="rId3" display="http://newon.docagent.net/" xr:uid="{1C652032-0C0E-495C-A381-6301BF9E6C79}"/>
+    <hyperlink ref="C4" r:id="rId4" display="http://newon.docagent.net/" xr:uid="{691E291D-9C87-4D2B-8FAE-6690B783690C}"/>
+    <hyperlink ref="C5" r:id="rId5" display="http://newon.docagent.net/" xr:uid="{1B6510E9-325A-4F65-A4F1-0D06D1DF2B3F}"/>
+    <hyperlink ref="C6" r:id="rId6" display="http://newon.docagent.net/" xr:uid="{01A4AADA-9594-4718-9F98-62868A7D03B4}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{E28C8817-EF91-48DC-9C34-7866572F46C8}"/>
+    <hyperlink ref="F4" r:id="rId8" xr:uid="{CFB3A187-DC01-4E7D-B8FC-CD25405015B5}"/>
+    <hyperlink ref="F5" r:id="rId9" xr:uid="{3D2143E0-EEB8-4011-9361-62BB5A2AD4B1}"/>
+    <hyperlink ref="F6" r:id="rId10" xr:uid="{C5F019B9-2CAC-41D1-A04F-4B8B5B2E027E}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>